<commit_message>
execute some test cases
</commit_message>
<xml_diff>
--- a/Guru99/TC_V2.xlsx
+++ b/Guru99/TC_V2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badri\Documents\GitHub\Manual-Testing\Guru99\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1977AD-D833-4802-BC5E-40F8AC3B5309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9A1E10-E60F-45F4-8069-5C61072BAA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13490" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="122">
   <si>
     <t>ID</t>
   </si>
@@ -780,6 +780,9 @@
 9) phone entered
 10) emailid entered
 11)unsuccefull message appear(email is invalid)</t>
+  </si>
+  <si>
+    <t>expected message "can not start with space", Actual "numbers are not allowed"</t>
   </si>
 </sst>
 </file>
@@ -1317,7 +1320,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -2324,8 +2327,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" colorId="8" zoomScale="55" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A22" colorId="8" zoomScale="87" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -2391,7 +2394,7 @@
       </c>
       <c r="B7" s="1">
         <f>COUNTIF(I:I, "pass")</f>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:10" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2485,7 +2488,7 @@
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="5" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2512,7 +2515,7 @@
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="5" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2539,7 +2542,7 @@
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="5" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2566,7 +2569,7 @@
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="5" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2591,7 +2594,7 @@
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="5" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="316.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2618,7 +2621,7 @@
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="5" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="316.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2645,7 +2648,7 @@
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="5" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="316.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2672,7 +2675,7 @@
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="5" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="316.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2697,9 +2700,11 @@
       <c r="G21" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="H21" s="10"/>
+      <c r="H21" s="10" t="s">
+        <v>121</v>
+      </c>
       <c r="I21" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="316.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2726,7 +2731,7 @@
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="5" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="316.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>